<commit_message>
Registry and Financial code updated
</commit_message>
<xml_diff>
--- a/Config/Australia_Financial_Config.xlsx
+++ b/Config/Australia_Financial_Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRADSOL123\PycharmProjects\MNS-Australia\MNS-Australia\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EB1A7F-1643-4969-931C-BCA6F62C32A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33411C6-156A-4708-B299-D854079892B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1245" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="447">
   <si>
     <t>Field_Name</t>
   </si>
@@ -1330,21 +1330,6 @@
   </si>
   <si>
     <t>profit_before_tax+profit_for_period_from_continuing_operations+profit_from_discontinuing_operation_after_tax-income_tax-Current_Tax-Deferred_Tax-Advance_Tax-Other_Tax_Expenses</t>
-  </si>
-  <si>
-    <t>Profit for period from continuing operations</t>
-  </si>
-  <si>
-    <t>Profit from discontinuing operation after tax</t>
-  </si>
-  <si>
-    <t>Current Tax</t>
-  </si>
-  <si>
-    <t>Advance Tax</t>
-  </si>
-  <si>
-    <t>Other Tax Expenses</t>
   </si>
   <si>
     <t>State_and_other_public_entities</t>
@@ -1798,8 +1783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
-      <selection activeCell="D262" sqref="D262"/>
+    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
+      <selection activeCell="A196" sqref="A196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,7 +2091,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>135</v>
@@ -2181,7 +2166,7 @@
         <v>136</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D20" t="s">
         <v>134</v>
@@ -2359,7 +2344,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>135</v>
@@ -2756,7 +2741,7 @@
         <v>136</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="D45" t="s">
         <v>134</v>
@@ -3187,7 +3172,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>135</v>
@@ -3233,7 +3218,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>135</v>
@@ -5060,13 +5045,13 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="B147" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D147" t="s">
         <v>134</v>
@@ -5087,7 +5072,7 @@
         <v>136</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="D148" t="s">
         <v>134</v>
@@ -5119,7 +5104,7 @@
         <v>136</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="D151" t="s">
         <v>134</v>
@@ -5935,7 +5920,7 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="6" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="B194" s="6" t="s">
         <v>135</v>
@@ -5981,7 +5966,7 @@
         <v>136</v>
       </c>
       <c r="C196" s="6" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="D196" t="s">
         <v>134</v>
@@ -6881,7 +6866,7 @@
         <v>136</v>
       </c>
       <c r="C241" s="6" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="D241" t="s">
         <v>134</v>
@@ -7161,7 +7146,7 @@
         <v>135</v>
       </c>
       <c r="C255" s="6" t="s">
-        <v>434</v>
+        <v>29</v>
       </c>
       <c r="D255" t="s">
         <v>134</v>
@@ -7181,7 +7166,7 @@
         <v>135</v>
       </c>
       <c r="C256" s="6" t="s">
-        <v>435</v>
+        <v>29</v>
       </c>
       <c r="D256" t="s">
         <v>134</v>
@@ -7201,7 +7186,7 @@
         <v>135</v>
       </c>
       <c r="C257" s="6" t="s">
-        <v>436</v>
+        <v>29</v>
       </c>
       <c r="D257" t="s">
         <v>134</v>
@@ -7221,7 +7206,7 @@
         <v>135</v>
       </c>
       <c r="C258" s="6" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
       <c r="D258" t="s">
         <v>134</v>
@@ -7241,7 +7226,7 @@
         <v>135</v>
       </c>
       <c r="C259" s="6" t="s">
-        <v>437</v>
+        <v>29</v>
       </c>
       <c r="D259" t="s">
         <v>134</v>
@@ -7261,7 +7246,7 @@
         <v>135</v>
       </c>
       <c r="C260" s="6" t="s">
-        <v>438</v>
+        <v>29</v>
       </c>
       <c r="D260" t="s">
         <v>134</v>
@@ -7301,7 +7286,7 @@
         <v>136</v>
       </c>
       <c r="C262" s="11" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="D262" t="s">
         <v>134</v>

</xml_diff>

<commit_message>
Code updated with client feedbacks
</commit_message>
<xml_diff>
--- a/Config/Australia_Financial_Config.xlsx
+++ b/Config/Australia_Financial_Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRADSOL123\PycharmProjects\MNS-Australia\MNS-Australia\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33411C6-156A-4708-B299-D854079892B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4841B725-2E51-4818-A85B-95C7D8B788BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1245" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$232</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$235</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1667" uniqueCount="454">
   <si>
     <t>Field_Name</t>
   </si>
@@ -915,9 +915,6 @@
     <t>investments_and_other_financial_assets_current</t>
   </si>
   <si>
-    <t>interest_bearing_liabilities+interest_bearing_liabilities_including_lease_liabilities+financial_liabilities</t>
-  </si>
-  <si>
     <t>investment+investments_and_other_financial_assets_current</t>
   </si>
   <si>
@@ -1221,9 +1218,6 @@
     <t>Repairs and maintenance expense</t>
   </si>
   <si>
-    <t>depreciation_and_amortisation_expenses+depreciation_and_amortisation_expense+depreciation_and_impairment_expenses+depreciation_and_impairment_expense+depreciation_property_plant_and_equipment+depreciation_ROU_assets</t>
-  </si>
-  <si>
     <t>depreciation_and_amortisation_expenses</t>
   </si>
   <si>
@@ -1356,9 +1350,6 @@
     <t>goodwill_and_intangible_assets+Intangible_assets+intangibles+goodwill</t>
   </si>
   <si>
-    <t>right_of_use+right_of_use_assets+other_receivables+other_non_financial_assets+other_non_current_assets+others_noncurrent+other_noncurrent</t>
-  </si>
-  <si>
     <t>Other_income</t>
   </si>
   <si>
@@ -1369,6 +1360,36 @@
   </si>
   <si>
     <t xml:space="preserve">net_revenue +other_income+Revenue_from_Service+Other_Operating_Revenue+ Subsidy_Income+ Financial_Income+ Gains_Losses_Allocated_Subsidiaries_Associates_Joint_Ventures+ Income_Loss_from_Discontinued_Operations+ Group_Contribution_Received+ Non_Operating_Income- total_cost_of_materials_consumed - Power_Fuel-total_purchases_of_stock_in_trade - total_changes_in_inventories_or_finished_goods - total_employee_benefit_expense - total_other_expenses - depreciation- selling_expenses - administration_costs - Advertising_expense- Services- Auditors_Fee- Management_Expenses- Legal_Professional_Charges - Other_General_Expense- Repair_of_Machinery-Personal_costs - Group_Contribution_Paid- Suppliers_And_External_Services- Impairment_Of_Investments_Not_Depreciable_Amortizable- interest - Other_Financial_Expenses + exceptional_items_before_tax  - income_tax - Current_Tax-Deferred_Tax -Advance_Tax-Other_Tax_Expenses+ profit_for_period_from_continuing_operations + profit_from_discontinuing_operation_after_tax - profit_after_tax </t>
+  </si>
+  <si>
+    <t>Assets held for sale</t>
+  </si>
+  <si>
+    <t>Assets_held_for_sale</t>
+  </si>
+  <si>
+    <t>right_of_use+right_of_use_assets+other_receivables+other_non_financial_assets+other_non_current_assets+others_noncurrent+other_noncurrent+Assets_held_for_sale</t>
+  </si>
+  <si>
+    <t>Related Party Loans</t>
+  </si>
+  <si>
+    <t>Related_Party_Loans</t>
+  </si>
+  <si>
+    <t>interest_bearing_liabilities+interest_bearing_liabilities_including_lease_liabilities+financial_liabilities+Related_Party_Loans</t>
+  </si>
+  <si>
+    <t>Changes in inventories of finished goods</t>
+  </si>
+  <si>
+    <t>Depreciation expenses</t>
+  </si>
+  <si>
+    <t>Depreciation_expenses</t>
+  </si>
+  <si>
+    <t>depreciation_and_amortisation_expenses+depreciation_and_amortisation_expense+depreciation_and_impairment_expenses+depreciation_and_impairment_expense+depreciation_property_plant_and_equipment+depreciation_ROU_assets+Depreciation_expenses</t>
   </si>
 </sst>
 </file>
@@ -1781,10 +1802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H262"/>
+  <dimension ref="A1:H265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
-      <selection activeCell="A196" sqref="A196"/>
+    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="C236" sqref="C236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1898,7 +1919,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>135</v>
@@ -1908,7 +1929,7 @@
         <v>134</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H7" t="s">
         <v>143</v>
@@ -2091,7 +2112,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>135</v>
@@ -2166,7 +2187,7 @@
         <v>136</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D20" t="s">
         <v>134</v>
@@ -2344,7 +2365,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>135</v>
@@ -2733,15 +2754,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>32</v>
+        <v>445</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="D45" t="s">
         <v>134</v>
@@ -2756,15 +2777,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>201</v>
+        <v>32</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>169</v>
+        <v>446</v>
       </c>
       <c r="D46" t="s">
         <v>134</v>
@@ -2773,21 +2794,21 @@
         <v>146</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H46" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>294</v>
+        <v>201</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D47" t="s">
         <v>134</v>
@@ -2804,13 +2825,13 @@
     </row>
     <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>33</v>
+        <v>294</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>296</v>
+        <v>162</v>
       </c>
       <c r="D48" t="s">
         <v>134</v>
@@ -2825,15 +2846,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>137</v>
+        <v>295</v>
       </c>
       <c r="D49" t="s">
         <v>134</v>
@@ -2850,13 +2871,13 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>219</v>
+        <v>34</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>220</v>
+        <v>137</v>
       </c>
       <c r="D50" t="s">
         <v>134</v>
@@ -2873,13 +2894,13 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>170</v>
+        <v>220</v>
       </c>
       <c r="D51" t="s">
         <v>134</v>
@@ -2896,13 +2917,13 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>221</v>
+        <v>170</v>
       </c>
       <c r="D52" t="s">
         <v>134</v>
@@ -2917,15 +2938,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>35</v>
+        <v>191</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D53" t="s">
         <v>134</v>
@@ -2940,15 +2961,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>29</v>
+        <v>218</v>
       </c>
       <c r="D54" t="s">
         <v>134</v>
@@ -2963,15 +2984,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>203</v>
+        <v>36</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>171</v>
+        <v>29</v>
       </c>
       <c r="D55" t="s">
         <v>134</v>
@@ -2988,13 +3009,13 @@
     </row>
     <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="D56" t="s">
         <v>134</v>
@@ -3010,14 +3031,14 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>136</v>
+      <c r="A57" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>222</v>
+        <v>139</v>
       </c>
       <c r="D57" t="s">
         <v>134</v>
@@ -3032,15 +3053,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>135</v>
+    <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>172</v>
+        <v>222</v>
       </c>
       <c r="D58" t="s">
         <v>134</v>
@@ -3057,13 +3078,13 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>194</v>
+        <v>38</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>31</v>
+        <v>172</v>
       </c>
       <c r="D59" t="s">
         <v>134</v>
@@ -3080,13 +3101,13 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>173</v>
+        <v>31</v>
       </c>
       <c r="D60" t="s">
         <v>134</v>
@@ -3103,13 +3124,13 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D61" t="s">
         <v>134</v>
@@ -3126,13 +3147,13 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>39</v>
+        <v>206</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>216</v>
+        <v>174</v>
       </c>
       <c r="D62" t="s">
         <v>134</v>
@@ -3149,13 +3170,13 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>29</v>
+        <v>216</v>
       </c>
       <c r="D63" t="s">
         <v>134</v>
@@ -3172,7 +3193,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>434</v>
+        <v>40</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>135</v>
@@ -3195,7 +3216,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>41</v>
+        <v>432</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>135</v>
@@ -3218,7 +3239,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>435</v>
+        <v>41</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>135</v>
@@ -3241,13 +3262,13 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>207</v>
+        <v>433</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>175</v>
+        <v>29</v>
       </c>
       <c r="D67" t="s">
         <v>134</v>
@@ -3264,13 +3285,13 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D68" t="s">
         <v>134</v>
@@ -3287,13 +3308,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D69" t="s">
         <v>134</v>
@@ -3308,15 +3329,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>42</v>
+        <v>209</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>217</v>
+        <v>177</v>
       </c>
       <c r="D70" t="s">
         <v>134</v>
@@ -3331,15 +3352,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>29</v>
+        <v>217</v>
       </c>
       <c r="D71" t="s">
         <v>134</v>
@@ -3356,13 +3377,13 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>178</v>
+        <v>29</v>
       </c>
       <c r="D72" t="s">
         <v>134</v>
@@ -3379,7 +3400,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>210</v>
+        <v>44</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>135</v>
@@ -3402,13 +3423,13 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D74" t="s">
         <v>134</v>
@@ -3425,13 +3446,13 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>291</v>
+        <v>211</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="D75" t="s">
         <v>134</v>
@@ -3448,13 +3469,13 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D76" t="s">
         <v>134</v>
@@ -3471,13 +3492,13 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>212</v>
+        <v>292</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="D77" t="s">
         <v>134</v>
@@ -3494,13 +3515,13 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>283</v>
+        <v>212</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D78" t="s">
         <v>134</v>
@@ -3517,13 +3538,13 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>213</v>
+        <v>283</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D79" t="s">
         <v>134</v>
@@ -3540,13 +3561,13 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D80" t="s">
         <v>134</v>
@@ -3561,15 +3582,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>45</v>
+        <v>214</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>293</v>
+        <v>183</v>
       </c>
       <c r="D81" t="s">
         <v>134</v>
@@ -3584,15 +3605,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>47</v>
+        <v>293</v>
       </c>
       <c r="D82" t="s">
         <v>134</v>
@@ -3600,55 +3621,55 @@
       <c r="E82" t="s">
         <v>146</v>
       </c>
-      <c r="F82" s="5"/>
+      <c r="F82" s="5" t="s">
+        <v>224</v>
+      </c>
       <c r="H82" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
+      <c r="A83" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D83" t="s">
+        <v>134</v>
+      </c>
+      <c r="E83" t="s">
+        <v>146</v>
+      </c>
+      <c r="F83" s="5"/>
+      <c r="H83" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="A84" s="5"/>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D85" t="s">
-        <v>134</v>
-      </c>
-      <c r="E85" t="s">
-        <v>147</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H85" t="s">
-        <v>153</v>
-      </c>
+      <c r="A85" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>279</v>
+        <v>225</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D86" t="s">
         <v>134</v>
@@ -3665,13 +3686,13 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>228</v>
+        <v>279</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D87" t="s">
         <v>134</v>
@@ -3688,13 +3709,13 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>49</v>
+        <v>228</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>280</v>
+        <v>229</v>
       </c>
       <c r="D88" t="s">
         <v>134</v>
@@ -3711,13 +3732,13 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>231</v>
+        <v>280</v>
       </c>
       <c r="D89" t="s">
         <v>134</v>
@@ -3734,13 +3755,13 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D90" t="s">
         <v>134</v>
@@ -3757,13 +3778,13 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>29</v>
+        <v>230</v>
       </c>
       <c r="D91" t="s">
         <v>134</v>
@@ -3778,9 +3799,9 @@
         <v>153</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>135</v>
@@ -3803,7 +3824,7 @@
     </row>
     <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>135</v>
@@ -3824,9 +3845,9 @@
         <v>153</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>135</v>
@@ -3849,7 +3870,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B95" s="6" t="s">
         <v>135</v>
@@ -3872,13 +3893,13 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>232</v>
+        <v>55</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>140</v>
+        <v>29</v>
       </c>
       <c r="D96" t="s">
         <v>134</v>
@@ -3887,21 +3908,21 @@
         <v>147</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H96" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>234</v>
+        <v>140</v>
       </c>
       <c r="D97" t="s">
         <v>134</v>
@@ -3916,15 +3937,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>174</v>
+        <v>234</v>
       </c>
       <c r="D98" t="s">
         <v>134</v>
@@ -3941,13 +3962,13 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
       <c r="B99" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>236</v>
+        <v>174</v>
       </c>
       <c r="D99" t="s">
         <v>134</v>
@@ -3964,13 +3985,13 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>205</v>
+        <v>235</v>
       </c>
       <c r="B100" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>173</v>
+        <v>236</v>
       </c>
       <c r="D100" t="s">
         <v>134</v>
@@ -3987,13 +4008,13 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>289</v>
+        <v>205</v>
       </c>
       <c r="B101" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>237</v>
+        <v>173</v>
       </c>
       <c r="D101" t="s">
         <v>134</v>
@@ -4008,15 +4029,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>56</v>
+        <v>289</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>290</v>
+        <v>237</v>
       </c>
       <c r="D102" t="s">
         <v>134</v>
@@ -4031,15 +4052,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
-        <v>239</v>
+        <v>56</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>240</v>
+        <v>290</v>
       </c>
       <c r="D103" t="s">
         <v>134</v>
@@ -4056,13 +4077,13 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B104" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D104" t="s">
         <v>134</v>
@@ -4079,13 +4100,13 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>57</v>
+        <v>241</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D105" t="s">
         <v>134</v>
@@ -4100,15 +4121,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>29</v>
+        <v>238</v>
       </c>
       <c r="D106" t="s">
         <v>134</v>
@@ -4123,15 +4144,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
-        <v>211</v>
+        <v>58</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>244</v>
+        <v>29</v>
       </c>
       <c r="D107" t="s">
         <v>134</v>
@@ -4148,13 +4169,13 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>245</v>
+        <v>211</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>141</v>
+        <v>244</v>
       </c>
       <c r="D108" t="s">
         <v>134</v>
@@ -4171,13 +4192,13 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B109" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>247</v>
+        <v>141</v>
       </c>
       <c r="D109" t="s">
         <v>134</v>
@@ -4194,13 +4215,13 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
-        <v>214</v>
+        <v>246</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D110" t="s">
         <v>134</v>
@@ -4217,13 +4238,13 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D111" t="s">
         <v>134</v>
@@ -4238,15 +4259,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
-        <v>59</v>
+        <v>249</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="D112" t="s">
         <v>134</v>
@@ -4261,15 +4282,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="D113" t="s">
         <v>134</v>
@@ -4286,13 +4307,13 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
-        <v>232</v>
+        <v>60</v>
       </c>
       <c r="B114" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>140</v>
+        <v>251</v>
       </c>
       <c r="D114" t="s">
         <v>134</v>
@@ -4301,21 +4322,21 @@
         <v>147</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H114" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B115" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>234</v>
+        <v>140</v>
       </c>
       <c r="D115" t="s">
         <v>134</v>
@@ -4330,15 +4351,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="B116" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="D116" t="s">
         <v>134</v>
@@ -4353,15 +4374,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
-        <v>61</v>
+        <v>252</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>295</v>
+        <v>253</v>
       </c>
       <c r="D117" t="s">
         <v>134</v>
@@ -4378,13 +4399,13 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
-        <v>254</v>
+        <v>448</v>
       </c>
       <c r="B118" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>255</v>
+        <v>447</v>
       </c>
       <c r="D118" t="s">
         <v>134</v>
@@ -4399,15 +4420,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
-        <v>256</v>
+        <v>61</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>257</v>
+        <v>449</v>
       </c>
       <c r="D119" t="s">
         <v>134</v>
@@ -4424,13 +4445,13 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
-        <v>281</v>
+        <v>254</v>
       </c>
       <c r="B120" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D120" t="s">
         <v>134</v>
@@ -4447,13 +4468,13 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
-        <v>62</v>
+        <v>256</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>282</v>
+        <v>257</v>
       </c>
       <c r="D121" t="s">
         <v>134</v>
@@ -4470,13 +4491,13 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
-        <v>63</v>
+        <v>281</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>29</v>
+        <v>258</v>
       </c>
       <c r="D122" t="s">
         <v>134</v>
@@ -4493,13 +4514,13 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>29</v>
+        <v>282</v>
       </c>
       <c r="D123" t="s">
         <v>134</v>
@@ -4516,7 +4537,7 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>135</v>
@@ -4539,13 +4560,13 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
-        <v>214</v>
+        <v>64</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>248</v>
+        <v>29</v>
       </c>
       <c r="D125" t="s">
         <v>134</v>
@@ -4562,13 +4583,13 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
-        <v>249</v>
+        <v>65</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>250</v>
+        <v>29</v>
       </c>
       <c r="D126" t="s">
         <v>134</v>
@@ -4585,13 +4606,13 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
-        <v>66</v>
+        <v>214</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="D127" t="s">
         <v>134</v>
@@ -4608,13 +4629,13 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
-        <v>67</v>
+        <v>249</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>29</v>
+        <v>250</v>
       </c>
       <c r="D128" t="s">
         <v>134</v>
@@ -4631,13 +4652,13 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>29</v>
+        <v>259</v>
       </c>
       <c r="D129" t="s">
         <v>134</v>
@@ -4654,7 +4675,7 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>135</v>
@@ -4677,13 +4698,13 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
-        <v>261</v>
+        <v>68</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>262</v>
+        <v>29</v>
       </c>
       <c r="D131" t="s">
         <v>134</v>
@@ -4700,13 +4721,13 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
-        <v>263</v>
+        <v>69</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>264</v>
+        <v>29</v>
       </c>
       <c r="D132" t="s">
         <v>134</v>
@@ -4723,13 +4744,13 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B133" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D133" t="s">
         <v>134</v>
@@ -4746,13 +4767,13 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
-        <v>70</v>
+        <v>263</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D134" t="s">
         <v>134</v>
@@ -4769,13 +4790,13 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
-        <v>71</v>
+        <v>265</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>29</v>
+        <v>266</v>
       </c>
       <c r="D135" t="s">
         <v>134</v>
@@ -4792,13 +4813,13 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>29</v>
+        <v>260</v>
       </c>
       <c r="D136" t="s">
         <v>134</v>
@@ -4815,7 +4836,7 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B137" s="6" t="s">
         <v>135</v>
@@ -4838,13 +4859,13 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
-        <v>274</v>
+        <v>72</v>
       </c>
       <c r="B138" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>267</v>
+        <v>29</v>
       </c>
       <c r="D138" t="s">
         <v>134</v>
@@ -4861,13 +4882,13 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
-        <v>268</v>
+        <v>73</v>
       </c>
       <c r="B139" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>269</v>
+        <v>29</v>
       </c>
       <c r="D139" t="s">
         <v>134</v>
@@ -4884,13 +4905,13 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
-        <v>213</v>
+        <v>274</v>
       </c>
       <c r="B140" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>182</v>
+        <v>267</v>
       </c>
       <c r="D140" t="s">
         <v>134</v>
@@ -4907,19 +4928,19 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B141" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D141" t="s">
         <v>134</v>
       </c>
       <c r="E141" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F141" s="5" t="s">
         <v>278</v>
@@ -4930,19 +4951,19 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
-        <v>272</v>
+        <v>213</v>
       </c>
       <c r="B142" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>273</v>
+        <v>182</v>
       </c>
       <c r="D142" t="s">
         <v>134</v>
       </c>
       <c r="E142" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F142" s="5" t="s">
         <v>278</v>
@@ -4953,13 +4974,13 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
-        <v>75</v>
+        <v>270</v>
       </c>
       <c r="B143" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="D143" t="s">
         <v>134</v>
@@ -4976,19 +4997,19 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
-        <v>211</v>
+        <v>272</v>
       </c>
       <c r="B144" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>244</v>
+        <v>273</v>
       </c>
       <c r="D144" t="s">
         <v>134</v>
       </c>
       <c r="E144" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F144" s="5" t="s">
         <v>278</v>
@@ -4999,19 +5020,19 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
-        <v>245</v>
+        <v>75</v>
       </c>
       <c r="B145" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>141</v>
+        <v>251</v>
       </c>
       <c r="D145" t="s">
         <v>134</v>
       </c>
       <c r="E145" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F145" s="5" t="s">
         <v>278</v>
@@ -5020,15 +5041,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
-        <v>74</v>
+        <v>211</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>275</v>
+        <v>244</v>
       </c>
       <c r="D146" t="s">
         <v>134</v>
@@ -5045,13 +5066,13 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
-        <v>438</v>
+        <v>245</v>
       </c>
       <c r="B147" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>438</v>
+        <v>141</v>
       </c>
       <c r="D147" t="s">
         <v>134</v>
@@ -5059,20 +5080,22 @@
       <c r="E147" t="s">
         <v>147</v>
       </c>
-      <c r="F147" s="5"/>
+      <c r="F147" s="5" t="s">
+        <v>278</v>
+      </c>
       <c r="H147" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B148" s="6" t="s">
         <v>136</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>439</v>
+        <v>275</v>
       </c>
       <c r="D148" t="s">
         <v>134</v>
@@ -5080,71 +5103,75 @@
       <c r="E148" t="s">
         <v>147</v>
       </c>
+      <c r="F148" s="5" t="s">
+        <v>278</v>
+      </c>
       <c r="H148" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A149" s="6"/>
-      <c r="B149" s="6"/>
-      <c r="C149" s="6"/>
+      <c r="A149" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C149" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="D149" t="s">
+        <v>134</v>
+      </c>
+      <c r="E149" t="s">
+        <v>147</v>
+      </c>
+      <c r="F149" s="5"/>
+      <c r="H149" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A150" s="7" t="s">
+      <c r="A150" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B150" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C150" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="D150" t="s">
+        <v>134</v>
+      </c>
+      <c r="E150" t="s">
+        <v>147</v>
+      </c>
+      <c r="H150" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" s="6"/>
+      <c r="B151" s="6"/>
+      <c r="C151" s="6"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B150" s="5"/>
-      <c r="C150" s="5"/>
-    </row>
-    <row r="151" spans="1:8" ht="210" x14ac:dyDescent="0.25">
-      <c r="A151" s="8" t="s">
+      <c r="B152" s="5"/>
+      <c r="C152" s="5"/>
+    </row>
+    <row r="153" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+      <c r="A153" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="B151" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C151" s="9" t="s">
-        <v>437</v>
-      </c>
-      <c r="D151" t="s">
-        <v>134</v>
-      </c>
-      <c r="E151" t="s">
-        <v>148</v>
-      </c>
-      <c r="H151" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A152" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B152" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C152" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D152" t="s">
-        <v>134</v>
-      </c>
-      <c r="E152" t="s">
-        <v>148</v>
-      </c>
-      <c r="H152" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" ht="180" x14ac:dyDescent="0.25">
-      <c r="A153" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="B153" s="6" t="s">
         <v>136</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>297</v>
+        <v>435</v>
       </c>
       <c r="D153" t="s">
         <v>134</v>
@@ -5158,13 +5185,13 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B154" s="6" t="s">
         <v>136</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D154" t="s">
         <v>134</v>
@@ -5176,137 +5203,137 @@
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A155" s="1"/>
-      <c r="B155" s="2"/>
-      <c r="C155" s="2"/>
+    <row r="155" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A155" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B155" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C155" s="9" t="s">
+        <v>296</v>
+      </c>
       <c r="D155" t="s">
         <v>134</v>
       </c>
+      <c r="E155" t="s">
+        <v>148</v>
+      </c>
+      <c r="H155" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A156" s="3" t="s">
+      <c r="A156" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B156" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C156" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D156" t="s">
+        <v>134</v>
+      </c>
+      <c r="E156" t="s">
+        <v>148</v>
+      </c>
+      <c r="H156" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A157" s="1"/>
+      <c r="B157" s="2"/>
+      <c r="C157" s="2"/>
+      <c r="D157" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B156" s="4"/>
-      <c r="C156" s="2"/>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A157" s="3" t="s">
+      <c r="B158" s="4"/>
+      <c r="C158" s="2"/>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B157" s="4"/>
-      <c r="C157" s="2"/>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A158" s="6" t="s">
+      <c r="B159" s="4"/>
+      <c r="C159" s="2"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A160" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="B160" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C160" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D160" t="s">
+        <v>134</v>
+      </c>
+      <c r="E160" t="s">
+        <v>149</v>
+      </c>
+      <c r="H160" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A161" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="B158" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C158" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D158" t="s">
-        <v>134</v>
-      </c>
-      <c r="E158" t="s">
-        <v>149</v>
-      </c>
-      <c r="H158" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A159" s="6" t="s">
+      <c r="B161" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C161" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="B159" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C159" s="6" t="s">
+      <c r="D161" t="s">
+        <v>134</v>
+      </c>
+      <c r="E161" t="s">
+        <v>149</v>
+      </c>
+      <c r="H161" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A162" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="D159" t="s">
-        <v>134</v>
-      </c>
-      <c r="E159" t="s">
-        <v>149</v>
-      </c>
-      <c r="H159" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A160" s="6" t="s">
+      <c r="B162" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C162" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="B160" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C160" s="6" t="s">
+      <c r="D162" t="s">
+        <v>134</v>
+      </c>
+      <c r="E162" t="s">
+        <v>149</v>
+      </c>
+      <c r="H162" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A163" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="D160" t="s">
-        <v>134</v>
-      </c>
-      <c r="E160" t="s">
-        <v>149</v>
-      </c>
-      <c r="H160" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A161" s="6" t="s">
+      <c r="B163" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C163" s="6" t="s">
         <v>306</v>
-      </c>
-      <c r="B161" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C161" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="D161" t="s">
-        <v>134</v>
-      </c>
-      <c r="E161" t="s">
-        <v>149</v>
-      </c>
-      <c r="H161" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A162" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="B162" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C162" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="D162" t="s">
-        <v>134</v>
-      </c>
-      <c r="E162" t="s">
-        <v>149</v>
-      </c>
-      <c r="H162" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A163" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B163" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C163" s="6" t="s">
-        <v>300</v>
       </c>
       <c r="D163" t="s">
         <v>134</v>
@@ -5320,93 +5347,93 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="B164" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C164" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D164" t="s">
+        <v>134</v>
+      </c>
+      <c r="E164" t="s">
+        <v>149</v>
+      </c>
+      <c r="H164" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A165" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B165" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C165" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="D165" t="s">
+        <v>134</v>
+      </c>
+      <c r="E165" t="s">
+        <v>149</v>
+      </c>
+      <c r="H165" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A166" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="B166" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C166" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="B164" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C164" s="6" t="s">
+      <c r="D166" t="s">
+        <v>134</v>
+      </c>
+      <c r="E166" t="s">
+        <v>149</v>
+      </c>
+      <c r="H166" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A167" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="D164" t="s">
-        <v>134</v>
-      </c>
-      <c r="E164" t="s">
-        <v>149</v>
-      </c>
-      <c r="H164" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A165" s="6" t="s">
+      <c r="B167" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C167" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B165" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C165" s="6" t="s">
+      <c r="D167" t="s">
+        <v>134</v>
+      </c>
+      <c r="E167" t="s">
+        <v>149</v>
+      </c>
+      <c r="H167" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A168" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="D165" t="s">
-        <v>134</v>
-      </c>
-      <c r="E165" t="s">
-        <v>149</v>
-      </c>
-      <c r="H165" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A166" s="6" t="s">
+      <c r="B168" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C168" s="6" t="s">
         <v>315</v>
-      </c>
-      <c r="B166" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C166" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="D166" t="s">
-        <v>134</v>
-      </c>
-      <c r="E166" t="s">
-        <v>149</v>
-      </c>
-      <c r="H166" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B167" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C167" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="D167" t="s">
-        <v>134</v>
-      </c>
-      <c r="E167" t="s">
-        <v>149</v>
-      </c>
-      <c r="H167" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A168" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B168" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C168" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="D168" t="s">
         <v>134</v>
@@ -5420,13 +5447,13 @@
     </row>
     <row r="169" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C169" s="6" t="s">
-        <v>29</v>
+        <v>309</v>
       </c>
       <c r="D169" t="s">
         <v>134</v>
@@ -5438,9 +5465,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B170" s="6" t="s">
         <v>135</v>
@@ -5458,55 +5485,55 @@
         <v>152</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B171" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C171" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D171" t="s">
+        <v>134</v>
+      </c>
+      <c r="E171" t="s">
+        <v>149</v>
+      </c>
+      <c r="H171" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A172" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B172" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C172" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="D172" t="s">
+        <v>134</v>
+      </c>
+      <c r="E172" t="s">
+        <v>149</v>
+      </c>
+      <c r="H172" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A173" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="B173" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C173" s="6" t="s">
         <v>318</v>
-      </c>
-      <c r="B171" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C171" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="D171" t="s">
-        <v>134</v>
-      </c>
-      <c r="E171" t="s">
-        <v>149</v>
-      </c>
-      <c r="H171" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A172" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="B172" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C172" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="D172" t="s">
-        <v>134</v>
-      </c>
-      <c r="E172" t="s">
-        <v>149</v>
-      </c>
-      <c r="H172" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A173" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B173" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C173" s="6" t="s">
-        <v>317</v>
       </c>
       <c r="D173" t="s">
         <v>134</v>
@@ -5520,113 +5547,113 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="B174" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C174" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D174" t="s">
+        <v>134</v>
+      </c>
+      <c r="E174" t="s">
+        <v>149</v>
+      </c>
+      <c r="H174" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A175" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B175" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C175" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D175" t="s">
+        <v>134</v>
+      </c>
+      <c r="E175" t="s">
+        <v>149</v>
+      </c>
+      <c r="H175" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A176" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B176" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C176" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="B174" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C174" s="6" t="s">
+      <c r="D176" t="s">
+        <v>134</v>
+      </c>
+      <c r="E176" t="s">
+        <v>149</v>
+      </c>
+      <c r="H176" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A177" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="D174" t="s">
-        <v>134</v>
-      </c>
-      <c r="E174" t="s">
-        <v>149</v>
-      </c>
-      <c r="H174" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A175" s="6" t="s">
+      <c r="B177" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C177" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="B175" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C175" s="6" t="s">
+      <c r="D177" t="s">
+        <v>134</v>
+      </c>
+      <c r="E177" t="s">
+        <v>149</v>
+      </c>
+      <c r="H177" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A178" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="D175" t="s">
-        <v>134</v>
-      </c>
-      <c r="E175" t="s">
-        <v>149</v>
-      </c>
-      <c r="H175" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A176" s="6" t="s">
+      <c r="B178" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C178" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="B176" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C176" s="6" t="s">
+      <c r="D178" t="s">
+        <v>134</v>
+      </c>
+      <c r="E178" t="s">
+        <v>149</v>
+      </c>
+      <c r="H178" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A179" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="D176" t="s">
-        <v>134</v>
-      </c>
-      <c r="E176" t="s">
-        <v>149</v>
-      </c>
-      <c r="H176" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="177" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A177" s="6" t="s">
+      <c r="B179" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C179" s="6" t="s">
         <v>329</v>
-      </c>
-      <c r="B177" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C177" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="D177" t="s">
-        <v>134</v>
-      </c>
-      <c r="E177" t="s">
-        <v>149</v>
-      </c>
-      <c r="H177" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A178" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="B178" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C178" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="D178" t="s">
-        <v>134</v>
-      </c>
-      <c r="E178" t="s">
-        <v>149</v>
-      </c>
-      <c r="H178" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A179" s="6" t="s">
-        <v>333</v>
-      </c>
-      <c r="B179" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C179" s="6" t="s">
-        <v>334</v>
       </c>
       <c r="D179" t="s">
         <v>134</v>
@@ -5640,13 +5667,13 @@
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="B180" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C180" s="6" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D180" t="s">
         <v>134</v>
@@ -5660,13 +5687,13 @@
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="6" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B181" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C181" s="6" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D181" t="s">
         <v>134</v>
@@ -5680,13 +5707,13 @@
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="6" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B182" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C182" s="6" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D182" t="s">
         <v>134</v>
@@ -5700,13 +5727,13 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="6" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="B183" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C183" s="6" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D183" t="s">
         <v>134</v>
@@ -5720,13 +5747,13 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="6" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B184" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C184" s="6" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D184" t="s">
         <v>134</v>
@@ -5740,13 +5767,13 @@
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="6" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="B185" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C185" s="6" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D185" t="s">
         <v>134</v>
@@ -5758,15 +5785,15 @@
         <v>152</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="6" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B186" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C186" s="6" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D186" t="s">
         <v>134</v>
@@ -5780,113 +5807,113 @@
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="B187" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C187" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="D187" t="s">
+        <v>134</v>
+      </c>
+      <c r="E187" t="s">
+        <v>149</v>
+      </c>
+      <c r="H187" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A188" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="B188" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C188" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="D188" t="s">
+        <v>134</v>
+      </c>
+      <c r="E188" t="s">
+        <v>149</v>
+      </c>
+      <c r="H188" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A189" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B189" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C189" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="B187" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C187" s="6" t="s">
+      <c r="D189" t="s">
+        <v>134</v>
+      </c>
+      <c r="E189" t="s">
+        <v>149</v>
+      </c>
+      <c r="H189" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A190" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="D187" t="s">
-        <v>134</v>
-      </c>
-      <c r="E187" t="s">
-        <v>149</v>
-      </c>
-      <c r="H187" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A188" s="6" t="s">
+      <c r="B190" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C190" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="B188" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C188" s="6" t="s">
+      <c r="D190" t="s">
+        <v>134</v>
+      </c>
+      <c r="E190" t="s">
+        <v>149</v>
+      </c>
+      <c r="H190" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A191" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B191" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C191" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="D191" t="s">
+        <v>134</v>
+      </c>
+      <c r="E191" t="s">
+        <v>149</v>
+      </c>
+      <c r="H191" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A192" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B192" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C192" s="6" t="s">
         <v>352</v>
-      </c>
-      <c r="D188" t="s">
-        <v>134</v>
-      </c>
-      <c r="E188" t="s">
-        <v>149</v>
-      </c>
-      <c r="H188" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="189" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A189" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B189" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C189" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="D189" t="s">
-        <v>134</v>
-      </c>
-      <c r="E189" t="s">
-        <v>149</v>
-      </c>
-      <c r="H189" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A190" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B190" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C190" s="6" t="s">
-        <v>353</v>
-      </c>
-      <c r="D190" t="s">
-        <v>134</v>
-      </c>
-      <c r="E190" t="s">
-        <v>149</v>
-      </c>
-      <c r="H190" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A191" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="B191" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C191" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="D191" t="s">
-        <v>134</v>
-      </c>
-      <c r="E191" t="s">
-        <v>149</v>
-      </c>
-      <c r="H191" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A192" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="B192" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C192" s="6" t="s">
-        <v>357</v>
       </c>
       <c r="D192" t="s">
         <v>134</v>
@@ -5900,13 +5927,13 @@
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="6" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B193" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C193" s="6" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="D193" t="s">
         <v>134</v>
@@ -5920,13 +5947,13 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="6" t="s">
-        <v>443</v>
+        <v>355</v>
       </c>
       <c r="B194" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C194" s="6" t="s">
-        <v>95</v>
+        <v>356</v>
       </c>
       <c r="D194" t="s">
         <v>134</v>
@@ -5940,13 +5967,13 @@
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B195" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C195" s="6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D195" t="s">
         <v>134</v>
@@ -5958,15 +5985,15 @@
         <v>152</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="6" t="s">
-        <v>94</v>
+        <v>440</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C196" s="6" t="s">
-        <v>444</v>
+        <v>95</v>
       </c>
       <c r="D196" t="s">
         <v>134</v>
@@ -5980,13 +6007,13 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="6" t="s">
-        <v>99</v>
+        <v>359</v>
       </c>
       <c r="B197" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C197" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D197" t="s">
         <v>134</v>
@@ -6000,47 +6027,47 @@
     </row>
     <row r="198" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B198" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C198" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="D198" t="s">
+        <v>134</v>
+      </c>
+      <c r="E198" t="s">
+        <v>149</v>
+      </c>
+      <c r="H198" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A199" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B199" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C199" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="D199" t="s">
+        <v>134</v>
+      </c>
+      <c r="E199" t="s">
+        <v>149</v>
+      </c>
+      <c r="H199" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A200" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="B198" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C198" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D198" t="s">
-        <v>134</v>
-      </c>
-      <c r="E198" t="s">
-        <v>149</v>
-      </c>
-      <c r="H198" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="199" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A199" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B199" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C199" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D199" t="s">
-        <v>134</v>
-      </c>
-      <c r="E199" t="s">
-        <v>149</v>
-      </c>
-      <c r="H199" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A200" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="B200" s="6" t="s">
         <v>135</v>
@@ -6058,9 +6085,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B201" s="6" t="s">
         <v>135</v>
@@ -6078,175 +6105,175 @@
         <v>152</v>
       </c>
     </row>
-    <row r="202" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B202" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C202" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D202" t="s">
+        <v>134</v>
+      </c>
+      <c r="E202" t="s">
+        <v>149</v>
+      </c>
+      <c r="H202" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A203" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B203" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C203" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D203" t="s">
+        <v>134</v>
+      </c>
+      <c r="E203" t="s">
+        <v>149</v>
+      </c>
+      <c r="H203" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A204" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="B204" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C204" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="B202" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C202" s="6" t="s">
+      <c r="D204" t="s">
+        <v>134</v>
+      </c>
+      <c r="E204" t="s">
+        <v>149</v>
+      </c>
+      <c r="H204" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A205" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="D202" t="s">
-        <v>134</v>
-      </c>
-      <c r="E202" t="s">
-        <v>149</v>
-      </c>
-      <c r="H202" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A203" s="6" t="s">
+      <c r="B205" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C205" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="B203" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C203" s="6" t="s">
+      <c r="D205" t="s">
+        <v>134</v>
+      </c>
+      <c r="E205" t="s">
+        <v>149</v>
+      </c>
+      <c r="H205" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A206" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="D203" t="s">
-        <v>134</v>
-      </c>
-      <c r="E203" t="s">
-        <v>149</v>
-      </c>
-      <c r="H203" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A204" s="6" t="s">
+      <c r="B206" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C206" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="B204" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C204" s="6" t="s">
+      <c r="D206" t="s">
+        <v>134</v>
+      </c>
+      <c r="E206" t="s">
+        <v>149</v>
+      </c>
+      <c r="H206" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A207" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="D204" t="s">
-        <v>134</v>
-      </c>
-      <c r="E204" t="s">
-        <v>149</v>
-      </c>
-      <c r="H204" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A205" s="6" t="s">
+      <c r="B207" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C207" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="B205" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C205" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="D205" t="s">
-        <v>134</v>
-      </c>
-      <c r="E205" t="s">
-        <v>149</v>
-      </c>
-      <c r="H205" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="206" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A206" s="6" t="s">
+      <c r="D207" t="s">
+        <v>134</v>
+      </c>
+      <c r="E207" t="s">
+        <v>149</v>
+      </c>
+      <c r="H207" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A208" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B206" s="6" t="s">
+      <c r="B208" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C206" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="D206" t="s">
-        <v>134</v>
-      </c>
-      <c r="E206" t="s">
-        <v>149</v>
-      </c>
-      <c r="H206" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="207" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A207" s="6" t="s">
+      <c r="C208" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="D208" t="s">
+        <v>134</v>
+      </c>
+      <c r="E208" t="s">
+        <v>149</v>
+      </c>
+      <c r="H208" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A209" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="B209" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C209" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="B207" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C207" s="6" t="s">
+      <c r="D209" t="s">
+        <v>134</v>
+      </c>
+      <c r="E209" t="s">
+        <v>149</v>
+      </c>
+      <c r="H209" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A210" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="D207" t="s">
-        <v>134</v>
-      </c>
-      <c r="E207" t="s">
-        <v>149</v>
-      </c>
-      <c r="H207" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A208" s="6" t="s">
+      <c r="B210" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C210" s="6" t="s">
         <v>375</v>
-      </c>
-      <c r="B208" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C208" s="6" t="s">
-        <v>376</v>
-      </c>
-      <c r="D208" t="s">
-        <v>134</v>
-      </c>
-      <c r="E208" t="s">
-        <v>149</v>
-      </c>
-      <c r="H208" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A209" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="B209" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C209" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="D209" t="s">
-        <v>134</v>
-      </c>
-      <c r="E209" t="s">
-        <v>149</v>
-      </c>
-      <c r="H209" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="210" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A210" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B210" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C210" s="6" t="s">
-        <v>372</v>
       </c>
       <c r="D210" t="s">
         <v>134</v>
@@ -6260,113 +6287,113 @@
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="B211" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C211" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="D211" t="s">
+        <v>134</v>
+      </c>
+      <c r="E211" t="s">
+        <v>149</v>
+      </c>
+      <c r="H211" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A212" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B212" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C212" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="D212" t="s">
+        <v>134</v>
+      </c>
+      <c r="E212" t="s">
+        <v>149</v>
+      </c>
+      <c r="H212" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A213" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="B213" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C213" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="B211" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C211" s="6" t="s">
+      <c r="D213" t="s">
+        <v>134</v>
+      </c>
+      <c r="E213" t="s">
+        <v>149</v>
+      </c>
+      <c r="H213" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A214" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="D211" t="s">
-        <v>134</v>
-      </c>
-      <c r="E211" t="s">
-        <v>149</v>
-      </c>
-      <c r="H211" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A212" s="6" t="s">
+      <c r="B214" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C214" s="6" t="s">
         <v>382</v>
       </c>
-      <c r="B212" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C212" s="6" t="s">
+      <c r="D214" t="s">
+        <v>134</v>
+      </c>
+      <c r="E214" t="s">
+        <v>149</v>
+      </c>
+      <c r="H214" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A215" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="D212" t="s">
-        <v>134</v>
-      </c>
-      <c r="E212" t="s">
-        <v>149</v>
-      </c>
-      <c r="H212" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="213" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A213" s="6" t="s">
+      <c r="B215" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C215" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="B213" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C213" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="D213" t="s">
-        <v>134</v>
-      </c>
-      <c r="E213" t="s">
-        <v>149</v>
-      </c>
-      <c r="H213" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="214" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A214" s="6" t="s">
+      <c r="D215" t="s">
+        <v>134</v>
+      </c>
+      <c r="E215" t="s">
+        <v>149</v>
+      </c>
+      <c r="H215" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A216" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B214" s="6" t="s">
+      <c r="B216" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C214" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="D214" t="s">
-        <v>134</v>
-      </c>
-      <c r="E214" t="s">
-        <v>149</v>
-      </c>
-      <c r="H214" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A215" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B215" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C215" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D215" t="s">
-        <v>134</v>
-      </c>
-      <c r="E215" t="s">
-        <v>149</v>
-      </c>
-      <c r="H215" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A216" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B216" s="6" t="s">
-        <v>135</v>
-      </c>
       <c r="C216" s="6" t="s">
-        <v>29</v>
+        <v>378</v>
       </c>
       <c r="D216" t="s">
         <v>134</v>
@@ -6380,13 +6407,13 @@
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B217" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C217" s="6" t="s">
-        <v>386</v>
+        <v>29</v>
       </c>
       <c r="D217" t="s">
         <v>134</v>
@@ -6400,7 +6427,7 @@
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B218" s="6" t="s">
         <v>135</v>
@@ -6420,13 +6447,13 @@
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="6" t="s">
-        <v>388</v>
+        <v>109</v>
       </c>
       <c r="B219" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C219" s="6" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D219" t="s">
         <v>134</v>
@@ -6440,13 +6467,13 @@
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="6" t="s">
-        <v>390</v>
+        <v>110</v>
       </c>
       <c r="B220" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C220" s="6" t="s">
-        <v>391</v>
+        <v>29</v>
       </c>
       <c r="D220" t="s">
         <v>134</v>
@@ -6460,13 +6487,13 @@
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="6" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B221" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C221" s="6" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D221" t="s">
         <v>134</v>
@@ -6480,13 +6507,13 @@
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="6" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B222" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C222" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="D222" t="s">
         <v>134</v>
@@ -6498,15 +6525,15 @@
         <v>152</v>
       </c>
     </row>
-    <row r="223" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="6" t="s">
-        <v>111</v>
+        <v>391</v>
       </c>
       <c r="B223" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C223" s="6" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="D223" t="s">
         <v>134</v>
@@ -6520,13 +6547,13 @@
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="6" t="s">
-        <v>112</v>
+        <v>393</v>
       </c>
       <c r="B224" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C224" s="6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D224" t="s">
         <v>134</v>
@@ -6540,13 +6567,13 @@
     </row>
     <row r="225" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A225" s="6" t="s">
-        <v>398</v>
+        <v>111</v>
       </c>
       <c r="B225" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C225" s="6" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="D225" t="s">
         <v>134</v>
@@ -6558,15 +6585,15 @@
         <v>152</v>
       </c>
     </row>
-    <row r="226" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="6" t="s">
-        <v>400</v>
+        <v>112</v>
       </c>
       <c r="B226" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C226" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="D226" t="s">
         <v>134</v>
@@ -6580,13 +6607,13 @@
     </row>
     <row r="227" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="6" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="B227" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C227" s="6" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="D227" t="s">
         <v>134</v>
@@ -6600,13 +6627,13 @@
     </row>
     <row r="228" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" s="6" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="B228" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C228" s="6" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="D228" t="s">
         <v>134</v>
@@ -6620,13 +6647,13 @@
     </row>
     <row r="229" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A229" s="6" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="B229" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C229" s="6" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="D229" t="s">
         <v>134</v>
@@ -6638,15 +6665,15 @@
         <v>152</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A230" s="6" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="B230" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C230" s="6" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="D230" t="s">
         <v>134</v>
@@ -6658,15 +6685,15 @@
         <v>152</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" s="6" t="s">
-        <v>113</v>
+        <v>404</v>
       </c>
       <c r="B231" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C231" s="6" t="s">
-        <v>397</v>
+        <v>405</v>
       </c>
       <c r="D231" t="s">
         <v>134</v>
@@ -6680,13 +6707,13 @@
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="6" t="s">
-        <v>114</v>
+        <v>406</v>
       </c>
       <c r="B232" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C232" s="6" t="s">
-        <v>29</v>
+        <v>407</v>
       </c>
       <c r="D232" t="s">
         <v>134</v>
@@ -6700,13 +6727,13 @@
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="6" t="s">
-        <v>115</v>
+        <v>452</v>
       </c>
       <c r="B233" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C233" s="6" t="s">
-        <v>29</v>
+        <v>451</v>
       </c>
       <c r="D233" t="s">
         <v>134</v>
@@ -6718,15 +6745,15 @@
         <v>152</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A234" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B234" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C234" s="6" t="s">
-        <v>29</v>
+        <v>453</v>
       </c>
       <c r="D234" t="s">
         <v>134</v>
@@ -6740,13 +6767,13 @@
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" s="6" t="s">
-        <v>411</v>
+        <v>114</v>
       </c>
       <c r="B235" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C235" s="6" t="s">
-        <v>412</v>
+        <v>29</v>
       </c>
       <c r="D235" t="s">
         <v>134</v>
@@ -6760,13 +6787,13 @@
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="6" t="s">
-        <v>413</v>
+        <v>115</v>
       </c>
       <c r="B236" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C236" s="6" t="s">
-        <v>414</v>
+        <v>29</v>
       </c>
       <c r="D236" t="s">
         <v>134</v>
@@ -6778,15 +6805,15 @@
         <v>152</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B237" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C237" s="6" t="s">
-        <v>410</v>
+        <v>29</v>
       </c>
       <c r="D237" t="s">
         <v>134</v>
@@ -6800,13 +6827,13 @@
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" s="6" t="s">
-        <v>96</v>
+        <v>409</v>
       </c>
       <c r="B238" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C238" s="6" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="D238" t="s">
         <v>134</v>
@@ -6820,13 +6847,13 @@
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" s="6" t="s">
-        <v>97</v>
+        <v>411</v>
       </c>
       <c r="B239" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C239" s="6" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D239" t="s">
         <v>134</v>
@@ -6838,15 +6865,15 @@
         <v>152</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A240" s="6" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="B240" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C240" s="6" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="D240" t="s">
         <v>134</v>
@@ -6858,15 +6885,15 @@
         <v>152</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="6" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="B241" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C241" s="6" t="s">
-        <v>445</v>
+        <v>413</v>
       </c>
       <c r="D241" t="s">
         <v>134</v>
@@ -6880,13 +6907,13 @@
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="6" t="s">
-        <v>150</v>
+        <v>97</v>
       </c>
       <c r="B242" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C242" s="6" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="D242" t="s">
         <v>134</v>
@@ -6900,13 +6927,13 @@
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="6" t="s">
-        <v>420</v>
+        <v>98</v>
       </c>
       <c r="B243" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C243" s="6" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="D243" t="s">
         <v>134</v>
@@ -6918,15 +6945,15 @@
         <v>152</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A244" s="6" t="s">
-        <v>422</v>
+        <v>118</v>
       </c>
       <c r="B244" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C244" s="6" t="s">
-        <v>151</v>
+        <v>442</v>
       </c>
       <c r="D244" t="s">
         <v>134</v>
@@ -6940,13 +6967,13 @@
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="6" t="s">
-        <v>423</v>
+        <v>150</v>
       </c>
       <c r="B245" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C245" s="6" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="D245" t="s">
         <v>134</v>
@@ -6958,15 +6985,15 @@
         <v>152</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="6" t="s">
-        <v>119</v>
+        <v>418</v>
       </c>
       <c r="B246" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C246" s="6" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D246" t="s">
         <v>134</v>
@@ -6980,93 +7007,93 @@
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="B247" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C247" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D247" t="s">
+        <v>134</v>
+      </c>
+      <c r="E247" t="s">
+        <v>149</v>
+      </c>
+      <c r="H247" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A248" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="B248" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C248" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="D248" t="s">
+        <v>134</v>
+      </c>
+      <c r="E248" t="s">
+        <v>149</v>
+      </c>
+      <c r="H248" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A249" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B249" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C249" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="D249" t="s">
+        <v>134</v>
+      </c>
+      <c r="E249" t="s">
+        <v>149</v>
+      </c>
+      <c r="H249" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A250" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B247" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C247" s="6" t="s">
+      <c r="B250" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C250" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D247" t="s">
-        <v>134</v>
-      </c>
-      <c r="E247" t="s">
-        <v>149</v>
-      </c>
-      <c r="H247" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="248" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A248" s="6" t="s">
+      <c r="D250" t="s">
+        <v>134</v>
+      </c>
+      <c r="E250" t="s">
+        <v>149</v>
+      </c>
+      <c r="H250" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A251" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B248" s="6" t="s">
+      <c r="B251" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C248" s="6" t="s">
+      <c r="C251" s="6" t="s">
         <v>122</v>
-      </c>
-      <c r="D248" t="s">
-        <v>134</v>
-      </c>
-      <c r="E248" t="s">
-        <v>149</v>
-      </c>
-      <c r="H248" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A249" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B249" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C249" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D249" t="s">
-        <v>134</v>
-      </c>
-      <c r="E249" t="s">
-        <v>149</v>
-      </c>
-      <c r="H249" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="250" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A250" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B250" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C250" s="6" t="s">
-        <v>425</v>
-      </c>
-      <c r="D250" t="s">
-        <v>134</v>
-      </c>
-      <c r="E250" t="s">
-        <v>149</v>
-      </c>
-      <c r="H250" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A251" s="6" t="s">
-        <v>427</v>
-      </c>
-      <c r="B251" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C251" s="6" t="s">
-        <v>428</v>
       </c>
       <c r="D251" t="s">
         <v>134</v>
@@ -7080,13 +7107,13 @@
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="6" t="s">
-        <v>429</v>
+        <v>123</v>
       </c>
       <c r="B252" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C252" s="6" t="s">
-        <v>430</v>
+        <v>29</v>
       </c>
       <c r="D252" t="s">
         <v>134</v>
@@ -7098,15 +7125,15 @@
         <v>152</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A253" s="6" t="s">
-        <v>431</v>
+        <v>124</v>
       </c>
       <c r="B253" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C253" s="6" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="D253" t="s">
         <v>134</v>
@@ -7118,12 +7145,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="254" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" s="6" t="s">
-        <v>125</v>
+        <v>425</v>
       </c>
       <c r="B254" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C254" s="6" t="s">
         <v>426</v>
@@ -7138,69 +7165,69 @@
         <v>152</v>
       </c>
     </row>
-    <row r="255" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="B255" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C255" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="D255" t="s">
+        <v>134</v>
+      </c>
+      <c r="E255" t="s">
+        <v>149</v>
+      </c>
+      <c r="H255" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A256" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="B256" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C256" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="D256" t="s">
+        <v>134</v>
+      </c>
+      <c r="E256" t="s">
+        <v>149</v>
+      </c>
+      <c r="H256" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A257" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B257" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C257" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="D257" t="s">
+        <v>134</v>
+      </c>
+      <c r="E257" t="s">
+        <v>149</v>
+      </c>
+      <c r="H257" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A258" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="B255" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C255" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D255" t="s">
-        <v>134</v>
-      </c>
-      <c r="E255" t="s">
-        <v>149</v>
-      </c>
-      <c r="H255" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="256" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A256" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B256" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C256" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D256" t="s">
-        <v>134</v>
-      </c>
-      <c r="E256" t="s">
-        <v>149</v>
-      </c>
-      <c r="H256" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A257" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B257" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C257" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D257" t="s">
-        <v>134</v>
-      </c>
-      <c r="E257" t="s">
-        <v>149</v>
-      </c>
-      <c r="H257" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A258" s="6" t="s">
-        <v>127</v>
       </c>
       <c r="B258" s="6" t="s">
         <v>135</v>
@@ -7218,9 +7245,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="6" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B259" s="6" t="s">
         <v>135</v>
@@ -7240,7 +7267,7 @@
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B260" s="6" t="s">
         <v>135</v>
@@ -7258,43 +7285,103 @@
         <v>152</v>
       </c>
     </row>
-    <row r="261" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B261" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C261" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D261" t="s">
+        <v>134</v>
+      </c>
+      <c r="E261" t="s">
+        <v>149</v>
+      </c>
+      <c r="H261" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A262" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B262" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C262" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D262" t="s">
+        <v>134</v>
+      </c>
+      <c r="E262" t="s">
+        <v>149</v>
+      </c>
+      <c r="H262" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A263" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B263" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C263" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D263" t="s">
+        <v>134</v>
+      </c>
+      <c r="E263" t="s">
+        <v>149</v>
+      </c>
+      <c r="H263" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A264" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B261" s="6" t="s">
+      <c r="B264" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C261" s="6" t="s">
-        <v>433</v>
-      </c>
-      <c r="D261" t="s">
-        <v>134</v>
-      </c>
-      <c r="E261" t="s">
-        <v>149</v>
-      </c>
-      <c r="H261" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="262" spans="1:8" ht="345" x14ac:dyDescent="0.25">
-      <c r="A262" s="1" t="s">
+      <c r="C264" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="D264" t="s">
+        <v>134</v>
+      </c>
+      <c r="E264" t="s">
+        <v>149</v>
+      </c>
+      <c r="H264" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" ht="345" x14ac:dyDescent="0.25">
+      <c r="A265" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B262" s="6" t="s">
+      <c r="B265" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C262" s="11" t="s">
-        <v>446</v>
-      </c>
-      <c r="D262" t="s">
-        <v>134</v>
-      </c>
-      <c r="E262" t="s">
-        <v>149</v>
-      </c>
-      <c r="H262" t="s">
+      <c r="C265" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="D265" t="s">
+        <v>134</v>
+      </c>
+      <c r="E265" t="s">
+        <v>149</v>
+      </c>
+      <c r="H265" t="s">
         <v>152</v>
       </c>
     </row>

</xml_diff>